<commit_message>
import de plusieurs UO en meme temps ok + creation d'UO vide possible
</commit_message>
<xml_diff>
--- a/excel/UO - Copie.xlsx
+++ b/excel/UO - Copie.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents_D\Teletravail\expleoWebsite\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30DEC8B9-67ED-4A86-A14B-C041B19364E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCF69F21-348E-40F8-9B72-6820E5569F6D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuille_UO" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="36">
   <si>
     <t>num_uo</t>
   </si>
@@ -530,10 +530,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:S6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -666,6 +666,242 @@
         <v>32</v>
       </c>
     </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3" t="s">
+        <v>24</v>
+      </c>
+      <c r="M3" t="s">
+        <v>25</v>
+      </c>
+      <c r="N3" t="s">
+        <v>26</v>
+      </c>
+      <c r="O3" s="2">
+        <v>43552</v>
+      </c>
+      <c r="P3" s="2">
+        <v>44438</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>33</v>
+      </c>
+      <c r="R3" t="s">
+        <v>35</v>
+      </c>
+      <c r="S3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K4" t="s">
+        <v>23</v>
+      </c>
+      <c r="L4" t="s">
+        <v>24</v>
+      </c>
+      <c r="M4" t="s">
+        <v>25</v>
+      </c>
+      <c r="N4" t="s">
+        <v>26</v>
+      </c>
+      <c r="O4" s="2">
+        <v>43552</v>
+      </c>
+      <c r="P4" s="2">
+        <v>44438</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>33</v>
+      </c>
+      <c r="R4" t="s">
+        <v>35</v>
+      </c>
+      <c r="S4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L5" t="s">
+        <v>24</v>
+      </c>
+      <c r="M5" t="s">
+        <v>25</v>
+      </c>
+      <c r="N5" t="s">
+        <v>26</v>
+      </c>
+      <c r="O5" s="2">
+        <v>43552</v>
+      </c>
+      <c r="P5" s="2">
+        <v>44438</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>33</v>
+      </c>
+      <c r="R5" t="s">
+        <v>35</v>
+      </c>
+      <c r="S5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" t="s">
+        <v>21</v>
+      </c>
+      <c r="J6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K6" t="s">
+        <v>23</v>
+      </c>
+      <c r="L6" t="s">
+        <v>24</v>
+      </c>
+      <c r="M6" t="s">
+        <v>25</v>
+      </c>
+      <c r="N6" t="s">
+        <v>26</v>
+      </c>
+      <c r="O6" s="2">
+        <v>43552</v>
+      </c>
+      <c r="P6" s="2">
+        <v>44438</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>33</v>
+      </c>
+      <c r="R6" t="s">
+        <v>35</v>
+      </c>
+      <c r="S6" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>